<commit_message>
46th Commit - 10th March 2023 - Modified Test Plan
</commit_message>
<xml_diff>
--- a/test_plan/i2c_verification_test_plan_v2.xlsx
+++ b/test_plan/i2c_verification_test_plan_v2.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\All Practice Projects\wb_i2c\test_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17842280-4901-4A47-B2E3-10ADAE0C7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D935FB4C-1856-4B40-B9E2-AAB355F62857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Report" sheetId="2" r:id="rId2"/>
     <sheet name="wb_reg" sheetId="3" r:id="rId3"/>
+    <sheet name="i2c" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t xml:space="preserve">Test Case Plan For I2C Protocol Verification                                                                </t>
   </si>
@@ -320,12 +321,79 @@
   <si>
     <t># Write to a value to one register at a time and check if any the other registers that should not get affected because of it is getting affected. Repeat this test for all the registers.</t>
   </si>
+  <si>
+    <t>i2c_transmit_receive_test</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Data Transmission</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+# Write random values to all available memory addresses in i2c subordinate.
+# Check if the wb_dat_i data is matched with the data being transmitted to the i2c subordinate.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Data Receieve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+# Read all the memory address of i2c subordinate.
+# Check if the wb_dat_o data is matched with the data received from i2c subordinate.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case Plan For Wishbone I2C Master Core Verification                                                                </t>
+  </si>
+  <si>
+    <t>i2c_slave_mem_walking_one_test</t>
+  </si>
+  <si>
+    <t>i2c_slave_mem_walking_zero_test</t>
+  </si>
+  <si>
+    <t># Initially set all the bits of all the memory registers to 0.
+# Transmit 1'b1 to a particular memory address's particular bit and expect all other bits to be remained 0 when receiving.
+# Repeat this for all the possible combinations.</t>
+  </si>
+  <si>
+    <t># Initially set all the bits of all the memory registers to 1.
+# Transmit 1'b1111_1110 to a particular memory address.
+# Repeat this for all the possible combinations.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +501,13 @@
       <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -726,21 +801,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -768,6 +828,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -779,12 +860,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1169,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,22 +1192,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1554,7 +1629,7 @@
       <c r="AG9" s="28"/>
       <c r="AH9" s="28"/>
     </row>
-    <row r="10" spans="1:34" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -1602,7 +1677,7 @@
       <c r="AG10" s="28"/>
       <c r="AH10" s="28"/>
     </row>
-    <row r="11" spans="1:34" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -1650,7 +1725,7 @@
       <c r="AG11" s="28"/>
       <c r="AH11" s="28"/>
     </row>
-    <row r="12" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -6769,8 +6844,8 @@
   </sheetPr>
   <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6794,22 +6869,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -6832,46 +6907,46 @@
       <c r="AH1" s="2"/>
     </row>
     <row r="2" spans="1:34" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="43" t="s">
+      <c r="L2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="38" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="1"/>
@@ -6896,100 +6971,100 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
+      <c r="A3" s="39">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="55" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48" t="s">
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="47"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" spans="1:34" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
+      <c r="A4" s="39">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="55" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="47"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" spans="1:34" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="39">
         <v>3</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="54" t="s">
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="47"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="1:34" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44">
+      <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="54" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="47"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="42"/>
     </row>
     <row r="7" spans="1:34" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -11089,4 +11164,197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3846CA-211C-4EB2-9B90-2000C5C5DAA2}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="91" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="39">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="42"/>
+    </row>
+    <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="39">
+        <v>2</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="42"/>
+    </row>
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="39">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="39">
+        <v>4</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
47th Commit - 11th May 2023 - Modified testbench and added assertions for stat and stop conditions
</commit_message>
<xml_diff>
--- a/test_plan/i2c_verification_test_plan_v2.xlsx
+++ b/test_plan/i2c_verification_test_plan_v2.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\All Practice Projects\wb_i2c\test_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D935FB4C-1856-4B40-B9E2-AAB355F62857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FBE60E-98B0-4AB3-989F-D8A01632C864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v1" sheetId="1" r:id="rId1"/>
-    <sheet name="Bug Report" sheetId="2" r:id="rId2"/>
-    <sheet name="wb_reg" sheetId="3" r:id="rId3"/>
-    <sheet name="i2c" sheetId="4" r:id="rId4"/>
+    <sheet name="final_testplan" sheetId="5" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId2"/>
+    <sheet name="Bug Report" sheetId="2" r:id="rId3"/>
+    <sheet name="wb_reg" sheetId="3" r:id="rId4"/>
+    <sheet name="i2c" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="81">
   <si>
     <t xml:space="preserve">Test Case Plan For I2C Protocol Verification                                                                </t>
   </si>
@@ -388,12 +389,352 @@
 # Transmit 1'b1111_1110 to a particular memory address.
 # Repeat this for all the possible combinations.</t>
   </si>
+  <si>
+    <t>i2c_start_condition_test</t>
+  </si>
+  <si>
+    <t>CHK</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>i2c_stop_condition_test</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Check if the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i2c_busy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bit of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> register gets </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>HIGH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> within 3 cycles after -
+sda gets </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LOW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when scl remains </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">HIGH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bit of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> register is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>HIGH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Check if the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>i2c_busy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bit of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> register gets </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LOW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> within 3 cycles after -
+sda gets </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>HIGH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when scl remains </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">HIGH </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>stop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bit of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> register is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>HIGH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>PRERlo, PRERhi, CTR, TXR, RXR, CR, SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CR, SR</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x00, 0x01, 0x02, 0x03, 0x04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +848,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -698,7 +1045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -860,6 +1207,27 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1162,6 +1530,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4499EED7-B453-4390-8A3E-2A0C5A7DB677}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="91" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="59">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="44"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="61"/>
+    </row>
+    <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="59">
+        <v>2</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="44"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="61"/>
+    </row>
+    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="59">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="56"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="44"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -6801,14 +7356,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6837,7 +7394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -11166,12 +11723,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3846CA-211C-4EB2-9B90-2000C5C5DAA2}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>